<commit_message>
Fixed integration of DH developments + other updates into H2 heavy scenario.
</commit_message>
<xml_diff>
--- a/src_files/data_files/unitdata_chp-units.xlsx
+++ b/src_files/data_files/unitdata_chp-units.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Backbone\backbone\north_european_model\src_files\data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\backbone\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F839351-9F64-4392-A5E6-DA68FF72DECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBC3E99-A403-4D0D-97CF-221EE07076CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitdata" sheetId="1" r:id="rId1"/>
     <sheet name="Remove_conventionalVersions" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">unitdata!$A$1:$L$153</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">unitdata!$A$1:$L$112</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="40">
   <si>
     <t>Generator_ID</t>
   </si>
@@ -112,9 +112,6 @@
   </si>
   <si>
     <t>Heat storage charger</t>
-  </si>
-  <si>
-    <t>H2 heavy</t>
   </si>
   <si>
     <t>capacity_output1</t>
@@ -352,32 +349,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L153"/>
+  <dimension ref="A1:L112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A143" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N13" sqref="N13"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H130" sqref="H130"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="11" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="8" max="11" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -386,28 +383,28 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -427,7 +424,7 @@
         <v>7929</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -447,7 +444,7 @@
         <v>7512</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -467,7 +464,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -484,7 +481,7 @@
         <v>23300</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -504,7 +501,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -524,7 +521,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -544,7 +541,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -564,7 +561,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -581,7 +578,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -598,7 +595,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -615,7 +612,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -635,7 +632,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -655,7 +652,7 @@
         <v>10650</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -672,7 +669,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -689,7 +686,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -709,7 +706,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -729,7 +726,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -746,7 +743,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -763,7 +760,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -780,7 +777,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -800,7 +797,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>16</v>
       </c>
@@ -820,7 +817,7 @@
         <v>2045</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -840,7 +837,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>16</v>
       </c>
@@ -857,7 +854,7 @@
         <v>4158</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>16</v>
       </c>
@@ -874,7 +871,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>17</v>
       </c>
@@ -894,7 +891,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>17</v>
       </c>
@@ -914,7 +911,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -931,7 +928,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -948,7 +945,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>20</v>
       </c>
@@ -965,7 +962,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -982,7 +979,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -999,7 +996,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>15</v>
       </c>
@@ -1016,7 +1013,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>16</v>
       </c>
@@ -1033,7 +1030,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>16</v>
       </c>
@@ -1050,7 +1047,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>17</v>
       </c>
@@ -1067,7 +1064,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>17</v>
       </c>
@@ -1084,7 +1081,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>18</v>
       </c>
@@ -1101,7 +1098,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -1118,7 +1115,7 @@
         <v>1998</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -1135,7 +1132,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>19</v>
       </c>
@@ -1152,7 +1149,7 @@
         <v>2120</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>18</v>
       </c>
@@ -1169,7 +1166,7 @@
         <v>16500</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>18</v>
       </c>
@@ -1189,7 +1186,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>18</v>
       </c>
@@ -1209,7 +1206,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -1229,7 +1226,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>18</v>
       </c>
@@ -1246,7 +1243,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>18</v>
       </c>
@@ -1263,7 +1260,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>18</v>
       </c>
@@ -1283,7 +1280,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>18</v>
       </c>
@@ -1303,7 +1300,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>18</v>
       </c>
@@ -1323,7 +1320,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>18</v>
       </c>
@@ -1340,7 +1337,7 @@
         <v>18000</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -1360,7 +1357,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>20</v>
       </c>
@@ -1377,7 +1374,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>20</v>
       </c>
@@ -1394,7 +1391,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>20</v>
       </c>
@@ -1414,7 +1411,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>20</v>
       </c>
@@ -1434,7 +1431,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>20</v>
       </c>
@@ -1451,7 +1448,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>20</v>
       </c>
@@ -1468,7 +1465,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>20</v>
       </c>
@@ -1485,7 +1482,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>20</v>
       </c>
@@ -1502,7 +1499,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>20</v>
       </c>
@@ -1519,7 +1516,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>20</v>
       </c>
@@ -1539,7 +1536,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>20</v>
       </c>
@@ -1559,7 +1556,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -1576,7 +1573,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>20</v>
       </c>
@@ -1593,7 +1590,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>20</v>
       </c>
@@ -1610,7 +1607,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>20</v>
       </c>
@@ -1630,7 +1627,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>19</v>
       </c>
@@ -1647,7 +1644,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>19</v>
       </c>
@@ -1664,7 +1661,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>19</v>
       </c>
@@ -1684,7 +1681,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>19</v>
       </c>
@@ -1704,7 +1701,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>19</v>
       </c>
@@ -1724,7 +1721,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>19</v>
       </c>
@@ -1741,7 +1738,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>19</v>
       </c>
@@ -1758,7 +1755,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>19</v>
       </c>
@@ -1775,7 +1772,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>19</v>
       </c>
@@ -1792,7 +1789,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>19</v>
       </c>
@@ -1812,7 +1809,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>19</v>
       </c>
@@ -1832,7 +1829,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>19</v>
       </c>
@@ -1852,7 +1849,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>19</v>
       </c>
@@ -1869,7 +1866,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>19</v>
       </c>
@@ -1886,7 +1883,7 @@
         <v>22000</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>15</v>
       </c>
@@ -1903,7 +1900,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>15</v>
       </c>
@@ -1923,7 +1920,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>15</v>
       </c>
@@ -1943,7 +1940,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>15</v>
       </c>
@@ -1960,7 +1957,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>15</v>
       </c>
@@ -1977,7 +1974,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>15</v>
       </c>
@@ -1994,7 +1991,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>15</v>
       </c>
@@ -2014,7 +2011,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>15</v>
       </c>
@@ -2034,7 +2031,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>15</v>
       </c>
@@ -2051,7 +2048,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>15</v>
       </c>
@@ -2068,7 +2065,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>16</v>
       </c>
@@ -2085,7 +2082,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>16</v>
       </c>
@@ -2105,7 +2102,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>16</v>
       </c>
@@ -2125,7 +2122,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>16</v>
       </c>
@@ -2142,7 +2139,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>16</v>
       </c>
@@ -2159,7 +2156,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>16</v>
       </c>
@@ -2176,7 +2173,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>16</v>
       </c>
@@ -2196,7 +2193,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>16</v>
       </c>
@@ -2216,7 +2213,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>16</v>
       </c>
@@ -2233,7 +2230,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>16</v>
       </c>
@@ -2250,7 +2247,7 @@
         <v>11000</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>17</v>
       </c>
@@ -2267,7 +2264,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>17</v>
       </c>
@@ -2287,7 +2284,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>17</v>
       </c>
@@ -2307,7 +2304,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>17</v>
       </c>
@@ -2324,7 +2321,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>17</v>
       </c>
@@ -2341,7 +2338,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>17</v>
       </c>
@@ -2358,7 +2355,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>17</v>
       </c>
@@ -2378,7 +2375,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>17</v>
       </c>
@@ -2398,7 +2395,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>17</v>
       </c>
@@ -2415,7 +2412,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>17</v>
       </c>
@@ -2432,755 +2429,10 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A113" t="s">
-        <v>18</v>
-      </c>
-      <c r="B113" t="s">
-        <v>5</v>
-      </c>
-      <c r="D113" t="s">
-        <v>24</v>
-      </c>
-      <c r="E113">
-        <v>2035</v>
-      </c>
-      <c r="H113">
-        <v>7929</v>
-      </c>
-      <c r="J113">
-        <v>7929</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A114" t="s">
-        <v>18</v>
-      </c>
-      <c r="B114" t="s">
-        <v>13</v>
-      </c>
-      <c r="D114" t="s">
-        <v>24</v>
-      </c>
-      <c r="E114">
-        <v>2035</v>
-      </c>
-      <c r="H114">
-        <v>3750</v>
-      </c>
-      <c r="J114">
-        <v>7512</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A115" t="s">
-        <v>18</v>
-      </c>
-      <c r="B115" t="s">
-        <v>14</v>
-      </c>
-      <c r="D115" t="s">
-        <v>24</v>
-      </c>
-      <c r="E115">
-        <v>2035</v>
-      </c>
-      <c r="H115">
-        <v>300</v>
-      </c>
-      <c r="J115">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>18</v>
-      </c>
-      <c r="B116" t="s">
-        <v>8</v>
-      </c>
-      <c r="D116" t="s">
-        <v>24</v>
-      </c>
-      <c r="E116">
-        <v>2035</v>
-      </c>
-      <c r="H116">
-        <v>23300</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
-        <v>20</v>
-      </c>
-      <c r="B117" t="s">
-        <v>5</v>
-      </c>
-      <c r="D117" t="s">
-        <v>24</v>
-      </c>
-      <c r="E117">
-        <v>2035</v>
-      </c>
-      <c r="H117">
-        <v>967</v>
-      </c>
-      <c r="J117">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A118" t="s">
-        <v>20</v>
-      </c>
-      <c r="B118" t="s">
-        <v>13</v>
-      </c>
-      <c r="D118" t="s">
-        <v>24</v>
-      </c>
-      <c r="E118">
-        <v>2035</v>
-      </c>
-      <c r="H118">
-        <v>600</v>
-      </c>
-      <c r="J118">
-        <v>1166</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A119" t="s">
-        <v>20</v>
-      </c>
-      <c r="B119" t="s">
-        <v>12</v>
-      </c>
-      <c r="D119" t="s">
-        <v>24</v>
-      </c>
-      <c r="E119">
-        <v>2035</v>
-      </c>
-      <c r="H119">
-        <v>900</v>
-      </c>
-      <c r="J119">
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
-        <v>20</v>
-      </c>
-      <c r="B120" t="s">
-        <v>14</v>
-      </c>
-      <c r="D120" t="s">
-        <v>24</v>
-      </c>
-      <c r="E120">
-        <v>2035</v>
-      </c>
-      <c r="H120">
-        <v>300</v>
-      </c>
-      <c r="J120">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
-        <v>20</v>
-      </c>
-      <c r="B121" t="s">
-        <v>8</v>
-      </c>
-      <c r="D121" t="s">
-        <v>24</v>
-      </c>
-      <c r="E121">
-        <v>2035</v>
-      </c>
-      <c r="H121">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
-        <v>20</v>
-      </c>
-      <c r="B122" t="s">
-        <v>7</v>
-      </c>
-      <c r="D122" t="s">
-        <v>24</v>
-      </c>
-      <c r="E122">
-        <v>2035</v>
-      </c>
-      <c r="H122">
-        <v>1300</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A123" t="s">
-        <v>20</v>
-      </c>
-      <c r="B123" t="s">
-        <v>9</v>
-      </c>
-      <c r="D123" t="s">
-        <v>24</v>
-      </c>
-      <c r="E123">
-        <v>2035</v>
-      </c>
-      <c r="H123">
-        <v>820</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>19</v>
-      </c>
-      <c r="B124" t="s">
-        <v>5</v>
-      </c>
-      <c r="D124" t="s">
-        <v>24</v>
-      </c>
-      <c r="E124">
-        <v>2035</v>
-      </c>
-      <c r="H124">
-        <v>960</v>
-      </c>
-      <c r="J124">
-        <v>960</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>19</v>
-      </c>
-      <c r="B125" t="s">
-        <v>13</v>
-      </c>
-      <c r="D125" t="s">
-        <v>24</v>
-      </c>
-      <c r="E125">
-        <v>2035</v>
-      </c>
-      <c r="H125">
-        <v>5300</v>
-      </c>
-      <c r="J125">
-        <v>10650</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>19</v>
-      </c>
-      <c r="B126" t="s">
-        <v>8</v>
-      </c>
-      <c r="D126" t="s">
-        <v>24</v>
-      </c>
-      <c r="E126">
-        <v>2035</v>
-      </c>
-      <c r="H126">
-        <v>11000</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A127" t="s">
-        <v>19</v>
-      </c>
-      <c r="B127" t="s">
-        <v>7</v>
-      </c>
-      <c r="D127" t="s">
-        <v>24</v>
-      </c>
-      <c r="E127">
-        <v>2035</v>
-      </c>
-      <c r="H127">
-        <v>22000</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>15</v>
-      </c>
-      <c r="B128" t="s">
-        <v>14</v>
-      </c>
-      <c r="D128" t="s">
-        <v>24</v>
-      </c>
-      <c r="E128">
-        <v>2035</v>
-      </c>
-      <c r="H128">
-        <v>70</v>
-      </c>
-      <c r="J128">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>15</v>
-      </c>
-      <c r="B129" t="s">
-        <v>12</v>
-      </c>
-      <c r="D129" t="s">
-        <v>24</v>
-      </c>
-      <c r="E129">
-        <v>2035</v>
-      </c>
-      <c r="H129">
-        <v>135</v>
-      </c>
-      <c r="J129">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>15</v>
-      </c>
-      <c r="B130" t="s">
-        <v>9</v>
-      </c>
-      <c r="D130" t="s">
-        <v>24</v>
-      </c>
-      <c r="E130">
-        <v>2035</v>
-      </c>
-      <c r="H130">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A131" t="s">
-        <v>15</v>
-      </c>
-      <c r="B131" t="s">
-        <v>7</v>
-      </c>
-      <c r="D131" t="s">
-        <v>24</v>
-      </c>
-      <c r="E131">
-        <v>2035</v>
-      </c>
-      <c r="H131">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A132" t="s">
-        <v>16</v>
-      </c>
-      <c r="B132" t="s">
-        <v>10</v>
-      </c>
-      <c r="D132" t="s">
-        <v>24</v>
-      </c>
-      <c r="E132">
-        <v>2035</v>
-      </c>
-      <c r="H132">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A133" t="s">
-        <v>16</v>
-      </c>
-      <c r="B133" t="s">
-        <v>14</v>
-      </c>
-      <c r="D133" t="s">
-        <v>24</v>
-      </c>
-      <c r="E133">
-        <v>2035</v>
-      </c>
-      <c r="H133">
-        <v>200</v>
-      </c>
-      <c r="J133">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A134" t="s">
-        <v>16</v>
-      </c>
-      <c r="B134" t="s">
-        <v>12</v>
-      </c>
-      <c r="D134" t="s">
-        <v>24</v>
-      </c>
-      <c r="E134">
-        <v>2035</v>
-      </c>
-      <c r="H134">
-        <v>1020</v>
-      </c>
-      <c r="J134">
-        <v>2045</v>
-      </c>
-    </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A135" t="s">
-        <v>16</v>
-      </c>
-      <c r="B135" t="s">
-        <v>13</v>
-      </c>
-      <c r="D135" t="s">
-        <v>24</v>
-      </c>
-      <c r="E135">
-        <v>2035</v>
-      </c>
-      <c r="H135">
-        <v>289</v>
-      </c>
-      <c r="J135">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A136" t="s">
-        <v>16</v>
-      </c>
-      <c r="B136" t="s">
-        <v>9</v>
-      </c>
-      <c r="D136" t="s">
-        <v>24</v>
-      </c>
-      <c r="E136">
-        <v>2035</v>
-      </c>
-      <c r="H136">
-        <v>4158</v>
-      </c>
-    </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A137" t="s">
-        <v>16</v>
-      </c>
-      <c r="B137" t="s">
-        <v>7</v>
-      </c>
-      <c r="D137" t="s">
-        <v>24</v>
-      </c>
-      <c r="E137">
-        <v>2035</v>
-      </c>
-      <c r="H137">
-        <v>12000</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
-        <v>17</v>
-      </c>
-      <c r="B138" t="s">
-        <v>14</v>
-      </c>
-      <c r="D138" t="s">
-        <v>24</v>
-      </c>
-      <c r="E138">
-        <v>2035</v>
-      </c>
-      <c r="H138">
-        <v>80</v>
-      </c>
-      <c r="J138">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A139" t="s">
-        <v>17</v>
-      </c>
-      <c r="B139" t="s">
-        <v>12</v>
-      </c>
-      <c r="D139" t="s">
-        <v>24</v>
-      </c>
-      <c r="E139">
-        <v>2035</v>
-      </c>
-      <c r="H139">
-        <v>360</v>
-      </c>
-      <c r="J139">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A140" t="s">
-        <v>17</v>
-      </c>
-      <c r="B140" t="s">
-        <v>9</v>
-      </c>
-      <c r="D140" t="s">
-        <v>24</v>
-      </c>
-      <c r="E140">
-        <v>2035</v>
-      </c>
-      <c r="H140">
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
-        <v>17</v>
-      </c>
-      <c r="B141" t="s">
-        <v>7</v>
-      </c>
-      <c r="D141" t="s">
-        <v>24</v>
-      </c>
-      <c r="E141">
-        <v>2035</v>
-      </c>
-      <c r="H141">
-        <v>2500</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
-        <v>20</v>
-      </c>
-      <c r="B142" t="s">
-        <v>22</v>
-      </c>
-      <c r="D142" t="s">
-        <v>24</v>
-      </c>
-      <c r="E142">
-        <v>2035</v>
-      </c>
-      <c r="H142">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
-        <v>20</v>
-      </c>
-      <c r="B143" t="s">
-        <v>23</v>
-      </c>
-      <c r="D143" t="s">
-        <v>24</v>
-      </c>
-      <c r="E143">
-        <v>2035</v>
-      </c>
-      <c r="H143">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
-        <v>15</v>
-      </c>
-      <c r="B144" t="s">
-        <v>22</v>
-      </c>
-      <c r="D144" t="s">
-        <v>24</v>
-      </c>
-      <c r="E144">
-        <v>2035</v>
-      </c>
-      <c r="H144">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
-        <v>15</v>
-      </c>
-      <c r="B145" t="s">
-        <v>23</v>
-      </c>
-      <c r="D145" t="s">
-        <v>24</v>
-      </c>
-      <c r="E145">
-        <v>2035</v>
-      </c>
-      <c r="H145">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
-        <v>16</v>
-      </c>
-      <c r="B146" t="s">
-        <v>22</v>
-      </c>
-      <c r="D146" t="s">
-        <v>24</v>
-      </c>
-      <c r="E146">
-        <v>2035</v>
-      </c>
-      <c r="H146">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
-        <v>16</v>
-      </c>
-      <c r="B147" t="s">
-        <v>23</v>
-      </c>
-      <c r="D147" t="s">
-        <v>24</v>
-      </c>
-      <c r="E147">
-        <v>2035</v>
-      </c>
-      <c r="H147">
-        <v>760</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
-        <v>17</v>
-      </c>
-      <c r="B148" t="s">
-        <v>22</v>
-      </c>
-      <c r="D148" t="s">
-        <v>24</v>
-      </c>
-      <c r="E148">
-        <v>2035</v>
-      </c>
-      <c r="H148">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
-        <v>17</v>
-      </c>
-      <c r="B149" t="s">
-        <v>23</v>
-      </c>
-      <c r="D149" t="s">
-        <v>24</v>
-      </c>
-      <c r="E149">
-        <v>2035</v>
-      </c>
-      <c r="H149">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
-        <v>18</v>
-      </c>
-      <c r="B150" t="s">
-        <v>22</v>
-      </c>
-      <c r="D150" t="s">
-        <v>24</v>
-      </c>
-      <c r="E150">
-        <v>2035</v>
-      </c>
-      <c r="H150">
-        <v>1998</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>18</v>
-      </c>
-      <c r="B151" t="s">
-        <v>23</v>
-      </c>
-      <c r="D151" t="s">
-        <v>24</v>
-      </c>
-      <c r="E151">
-        <v>2035</v>
-      </c>
-      <c r="H151">
-        <v>1998</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
-        <v>19</v>
-      </c>
-      <c r="B152" t="s">
-        <v>22</v>
-      </c>
-      <c r="D152" t="s">
-        <v>24</v>
-      </c>
-      <c r="E152">
-        <v>2035</v>
-      </c>
-      <c r="H152">
-        <v>2120</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
-        <v>19</v>
-      </c>
-      <c r="B153" t="s">
-        <v>23</v>
-      </c>
-      <c r="D153" t="s">
-        <v>24</v>
-      </c>
-      <c r="E153">
-        <v>2035</v>
-      </c>
-      <c r="H153">
-        <v>2120</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:L153" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:L112" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:L112">
-      <sortCondition ref="A1:A153"/>
+      <sortCondition ref="A1:A112"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -3200,20 +2452,20 @@
       <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.6640625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="20" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" style="3"/>
+    <col min="5" max="5" width="11.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -3225,96 +2477,96 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="E2" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>21</v>

</xml_diff>